<commit_message>
Se cargó la información adicional en el formato de Recoleccion
</commit_message>
<xml_diff>
--- a/FormatoRecoleccionV2.xlsx
+++ b/FormatoRecoleccionV2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\InfnITSolutions\OneCarrier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3B86A7-D00C-466C-9308-07644EB33CBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7377548A-2C2E-44BE-86B0-7E4F3350841F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="6225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="154">
   <si>
     <t>ORDEN DE RECOLECCIÓN</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t>@content@'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InfAdicional @ </t>
   </si>
 </sst>
 </file>
@@ -2664,38 +2667,224 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2703,80 +2892,41 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="130" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="125" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2805,7 +2955,13 @@
     <xf numFmtId="0" fontId="22" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2841,7 +2997,19 @@
     <xf numFmtId="0" fontId="22" fillId="3" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2852,9 +3020,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2876,24 +3041,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="128" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2928,17 +3075,56 @@
     <xf numFmtId="0" fontId="22" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="128" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2952,38 +3138,41 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="130" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="125" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3001,63 +3190,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3090,131 +3222,159 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="115" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="73"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3233,263 +3393,64 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="73"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="15" fillId="10" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="8" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3511,38 +3472,80 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="15" fillId="10" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3867,8 +3870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3900,18 +3903,18 @@
     </row>
     <row r="2" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
-      <c r="C2" s="305" t="s">
+      <c r="C2" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="306"/>
-      <c r="E2" s="306"/>
-      <c r="F2" s="306"/>
-      <c r="G2" s="306"/>
-      <c r="H2" s="306"/>
-      <c r="I2" s="306"/>
-      <c r="J2" s="306"/>
-      <c r="K2" s="306"/>
-      <c r="L2" s="307"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="146"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
@@ -3958,33 +3961,33 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="308" t="s">
+      <c r="B6" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="309"/>
-      <c r="D6" s="310"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="149"/>
       <c r="E6" s="2"/>
       <c r="F6" s="98"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="248" t="s">
+      <c r="J6" s="193" t="s">
         <v>150</v>
       </c>
-      <c r="K6" s="248"/>
-      <c r="L6" s="248"/>
-      <c r="M6" s="248"/>
+      <c r="K6" s="193"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="193"/>
       <c r="N6" s="88"/>
     </row>
     <row r="7" spans="2:14" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="135" t="s">
+      <c r="B7" s="300" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="136"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="311"/>
-      <c r="F7" s="312"/>
-      <c r="G7" s="313"/>
+      <c r="C7" s="301"/>
+      <c r="D7" s="302"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="152"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -3996,23 +3999,23 @@
     <row r="8" spans="2:14" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
-      <c r="E8" s="314"/>
-      <c r="F8" s="314"/>
-      <c r="G8" s="314"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="153"/>
+      <c r="G8" s="153"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="315" t="s">
+      <c r="J8" s="154" t="s">
         <v>107</v>
       </c>
-      <c r="K8" s="316"/>
-      <c r="L8" s="316"/>
-      <c r="M8" s="316"/>
-      <c r="N8" s="317"/>
+      <c r="K8" s="155"/>
+      <c r="L8" s="155"/>
+      <c r="M8" s="155"/>
+      <c r="N8" s="156"/>
     </row>
     <row r="9" spans="2:14" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="87"/>
-      <c r="C9" s="318"/>
-      <c r="D9" s="318"/>
+      <c r="C9" s="135"/>
+      <c r="D9" s="135"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -4025,96 +4028,96 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="325" t="s">
+      <c r="B10" s="142" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="245" t="s">
+      <c r="C10" s="315" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="246"/>
-      <c r="E10" s="246"/>
-      <c r="F10" s="246"/>
-      <c r="G10" s="247"/>
+      <c r="D10" s="316"/>
+      <c r="E10" s="316"/>
+      <c r="F10" s="316"/>
+      <c r="G10" s="317"/>
       <c r="H10" s="6"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="319" t="s">
+      <c r="J10" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="320"/>
-      <c r="L10" s="320"/>
-      <c r="M10" s="320"/>
-      <c r="N10" s="321"/>
+      <c r="K10" s="137"/>
+      <c r="L10" s="137"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="138"/>
     </row>
     <row r="11" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="326"/>
-      <c r="C11" s="242" t="s">
+      <c r="B11" s="143"/>
+      <c r="C11" s="312" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="243"/>
-      <c r="E11" s="243"/>
-      <c r="F11" s="243"/>
-      <c r="G11" s="244"/>
+      <c r="D11" s="313"/>
+      <c r="E11" s="313"/>
+      <c r="F11" s="313"/>
+      <c r="G11" s="314"/>
       <c r="H11" s="6"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="322">
+      <c r="J11" s="139">
         <v>1</v>
       </c>
-      <c r="K11" s="323"/>
-      <c r="L11" s="323"/>
-      <c r="M11" s="323"/>
-      <c r="N11" s="324"/>
+      <c r="K11" s="140"/>
+      <c r="L11" s="140"/>
+      <c r="M11" s="140"/>
+      <c r="N11" s="141"/>
     </row>
     <row r="12" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="279" t="s">
+      <c r="B12" s="168" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="280"/>
-      <c r="D12" s="280"/>
-      <c r="E12" s="282"/>
-      <c r="F12" s="300" t="s">
+      <c r="C12" s="169"/>
+      <c r="D12" s="169"/>
+      <c r="E12" s="170"/>
+      <c r="F12" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="301"/>
+      <c r="G12" s="172"/>
       <c r="H12" s="5"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="302" t="s">
+      <c r="J12" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="303"/>
-      <c r="L12" s="303"/>
-      <c r="M12" s="303"/>
-      <c r="N12" s="304"/>
+      <c r="K12" s="203"/>
+      <c r="L12" s="203"/>
+      <c r="M12" s="203"/>
+      <c r="N12" s="204"/>
     </row>
     <row r="13" spans="2:14" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="273" t="s">
+      <c r="B13" s="324" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="258"/>
-      <c r="D13" s="258"/>
-      <c r="E13" s="274"/>
-      <c r="F13" s="275" t="s">
+      <c r="C13" s="184"/>
+      <c r="D13" s="184"/>
+      <c r="E13" s="325"/>
+      <c r="F13" s="326" t="s">
         <v>112</v>
       </c>
-      <c r="G13" s="276"/>
+      <c r="G13" s="327"/>
       <c r="H13" s="91"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="489" t="s">
+      <c r="J13" s="199" t="s">
         <v>152</v>
       </c>
-      <c r="K13" s="277"/>
-      <c r="L13" s="277"/>
-      <c r="M13" s="277"/>
-      <c r="N13" s="278"/>
+      <c r="K13" s="200"/>
+      <c r="L13" s="200"/>
+      <c r="M13" s="200"/>
+      <c r="N13" s="201"/>
     </row>
     <row r="14" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="279" t="s">
+      <c r="B14" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="280"/>
-      <c r="D14" s="280"/>
-      <c r="E14" s="280"/>
-      <c r="F14" s="280"/>
-      <c r="G14" s="281"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="169"/>
+      <c r="E14" s="169"/>
+      <c r="F14" s="169"/>
+      <c r="G14" s="177"/>
       <c r="H14" s="6"/>
       <c r="I14" s="95" t="s">
         <v>12</v>
@@ -4136,14 +4139,14 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="260" t="s">
+      <c r="B15" s="173" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="261"/>
-      <c r="D15" s="261"/>
-      <c r="E15" s="261"/>
-      <c r="F15" s="261"/>
-      <c r="G15" s="262"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="174"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="175"/>
       <c r="H15" s="6"/>
       <c r="I15" s="9">
         <v>1</v>
@@ -4165,16 +4168,16 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="279" t="s">
+      <c r="B16" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="280"/>
-      <c r="D16" s="280"/>
-      <c r="E16" s="282"/>
-      <c r="F16" s="283" t="s">
+      <c r="C16" s="169"/>
+      <c r="D16" s="169"/>
+      <c r="E16" s="170"/>
+      <c r="F16" s="176" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="281"/>
+      <c r="G16" s="177"/>
       <c r="H16" s="6"/>
       <c r="I16" s="9"/>
       <c r="J16" s="13"/>
@@ -4184,16 +4187,16 @@
       <c r="N16" s="12"/>
     </row>
     <row r="17" spans="2:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="284" t="s">
+      <c r="B17" s="178" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="285"/>
-      <c r="D17" s="285"/>
-      <c r="E17" s="286"/>
-      <c r="F17" s="287" t="s">
+      <c r="C17" s="179"/>
+      <c r="D17" s="179"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="181" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="288"/>
+      <c r="G17" s="182"/>
       <c r="H17" s="90"/>
       <c r="I17" s="14"/>
       <c r="J17" s="15"/>
@@ -4203,14 +4206,14 @@
       <c r="N17" s="16"/>
     </row>
     <row r="18" spans="2:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="289" t="s">
+      <c r="B18" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="290"/>
-      <c r="D18" s="290"/>
-      <c r="E18" s="290"/>
-      <c r="F18" s="290"/>
-      <c r="G18" s="291"/>
+      <c r="C18" s="158"/>
+      <c r="D18" s="158"/>
+      <c r="E18" s="158"/>
+      <c r="F18" s="158"/>
+      <c r="G18" s="159"/>
       <c r="H18" s="5"/>
       <c r="I18" s="14"/>
       <c r="J18" s="104"/>
@@ -4220,14 +4223,14 @@
       <c r="N18" s="16"/>
     </row>
     <row r="19" spans="2:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="297" t="s">
+      <c r="B19" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="298"/>
-      <c r="D19" s="298"/>
-      <c r="E19" s="298"/>
-      <c r="F19" s="298"/>
-      <c r="G19" s="299"/>
+      <c r="C19" s="166"/>
+      <c r="D19" s="166"/>
+      <c r="E19" s="166"/>
+      <c r="F19" s="166"/>
+      <c r="G19" s="167"/>
       <c r="H19" s="89"/>
       <c r="I19" s="21"/>
       <c r="J19" s="105"/>
@@ -4237,16 +4240,16 @@
       <c r="N19" s="100"/>
     </row>
     <row r="20" spans="2:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="292" t="s">
+      <c r="B20" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="293"/>
-      <c r="D20" s="293"/>
-      <c r="E20" s="294"/>
-      <c r="F20" s="295" t="s">
+      <c r="C20" s="161"/>
+      <c r="D20" s="161"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="163" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="296"/>
+      <c r="G20" s="164"/>
       <c r="H20" s="6"/>
       <c r="I20" s="101"/>
       <c r="J20" s="105"/>
@@ -4256,16 +4259,16 @@
       <c r="N20" s="103"/>
     </row>
     <row r="21" spans="2:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="270" t="s">
+      <c r="B21" s="321" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="165"/>
-      <c r="D21" s="165"/>
-      <c r="E21" s="166"/>
-      <c r="F21" s="271" t="s">
+      <c r="C21" s="257"/>
+      <c r="D21" s="257"/>
+      <c r="E21" s="287"/>
+      <c r="F21" s="322" t="s">
         <v>116</v>
       </c>
-      <c r="G21" s="272"/>
+      <c r="G21" s="323"/>
       <c r="H21" s="92"/>
       <c r="I21" s="115"/>
       <c r="J21" s="110"/>
@@ -4275,12 +4278,12 @@
       <c r="N21" s="110"/>
     </row>
     <row r="22" spans="2:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="267" t="s">
+      <c r="B22" s="318" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="268"/>
-      <c r="D22" s="268"/>
-      <c r="E22" s="269"/>
+      <c r="C22" s="319"/>
+      <c r="D22" s="319"/>
+      <c r="E22" s="320"/>
       <c r="F22" s="93" t="s">
         <v>25</v>
       </c>
@@ -4295,12 +4298,12 @@
       <c r="O22" s="116"/>
     </row>
     <row r="23" spans="2:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="227" t="s">
+      <c r="B23" s="296" t="s">
         <v>108</v>
       </c>
-      <c r="C23" s="228"/>
-      <c r="D23" s="228"/>
-      <c r="E23" s="149"/>
+      <c r="C23" s="297"/>
+      <c r="D23" s="297"/>
+      <c r="E23" s="223"/>
       <c r="F23" s="117" t="s">
         <v>109</v>
       </c>
@@ -4319,10 +4322,10 @@
         <v>122</v>
       </c>
       <c r="C24" s="120"/>
-      <c r="D24" s="150" t="s">
+      <c r="D24" s="308" t="s">
         <v>124</v>
       </c>
-      <c r="E24" s="151"/>
+      <c r="E24" s="309"/>
       <c r="F24" s="121" t="s">
         <v>126</v>
       </c>
@@ -4336,18 +4339,18 @@
       <c r="N24" s="129"/>
     </row>
     <row r="25" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="152" t="s">
+      <c r="B25" s="310" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="153"/>
-      <c r="D25" s="148" t="s">
+      <c r="C25" s="311"/>
+      <c r="D25" s="222" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="149"/>
-      <c r="F25" s="146" t="s">
+      <c r="E25" s="223"/>
+      <c r="F25" s="216" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="147"/>
+      <c r="G25" s="217"/>
       <c r="H25" s="5"/>
       <c r="I25" s="128"/>
       <c r="J25" s="99"/>
@@ -4359,58 +4362,58 @@
     </row>
     <row r="26" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H26" s="5"/>
-      <c r="I26" s="235" t="s">
+      <c r="I26" s="209" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="236"/>
-      <c r="K26" s="235" t="s">
+      <c r="J26" s="210"/>
+      <c r="K26" s="209" t="s">
         <v>118</v>
       </c>
-      <c r="L26" s="239"/>
-      <c r="M26" s="231"/>
-      <c r="N26" s="232"/>
+      <c r="L26" s="213"/>
+      <c r="M26" s="205"/>
+      <c r="N26" s="206"/>
     </row>
     <row r="27" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="144" t="s">
+      <c r="B27" s="306" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="138" t="s">
+      <c r="C27" s="303" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="139"/>
-      <c r="E27" s="139"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="140"/>
+      <c r="D27" s="304"/>
+      <c r="E27" s="304"/>
+      <c r="F27" s="304"/>
+      <c r="G27" s="305"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="237" t="s">
+      <c r="I27" s="211" t="s">
         <v>121</v>
       </c>
-      <c r="J27" s="238"/>
-      <c r="K27" s="240" t="s">
+      <c r="J27" s="212"/>
+      <c r="K27" s="214" t="s">
         <v>119</v>
       </c>
-      <c r="L27" s="241"/>
-      <c r="M27" s="233"/>
-      <c r="N27" s="234"/>
+      <c r="L27" s="215"/>
+      <c r="M27" s="207"/>
+      <c r="N27" s="208"/>
     </row>
     <row r="28" spans="2:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="145"/>
-      <c r="C28" s="141"/>
-      <c r="D28" s="142"/>
-      <c r="E28" s="142"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="143"/>
+      <c r="B28" s="307"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="225"/>
+      <c r="E28" s="225"/>
+      <c r="F28" s="225"/>
+      <c r="G28" s="187"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="266" t="s">
+      <c r="I28" s="198" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="190" t="s">
+      <c r="J28" s="249" t="s">
         <v>117</v>
       </c>
-      <c r="K28" s="191"/>
-      <c r="L28" s="191"/>
-      <c r="M28" s="191"/>
-      <c r="N28" s="192"/>
+      <c r="K28" s="250"/>
+      <c r="L28" s="250"/>
+      <c r="M28" s="250"/>
+      <c r="N28" s="251"/>
     </row>
     <row r="29" spans="2:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="123" t="s">
@@ -4419,17 +4422,19 @@
       <c r="C29" s="124" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="212"/>
-      <c r="E29" s="213"/>
-      <c r="F29" s="213"/>
-      <c r="G29" s="214"/>
+      <c r="D29" s="268" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="269"/>
+      <c r="F29" s="269"/>
+      <c r="G29" s="270"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="252"/>
-      <c r="J29" s="141"/>
-      <c r="K29" s="142"/>
-      <c r="L29" s="142"/>
-      <c r="M29" s="142"/>
-      <c r="N29" s="193"/>
+      <c r="I29" s="197"/>
+      <c r="J29" s="186"/>
+      <c r="K29" s="225"/>
+      <c r="L29" s="225"/>
+      <c r="M29" s="225"/>
+      <c r="N29" s="252"/>
     </row>
     <row r="30" spans="2:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="123" t="s">
@@ -4438,318 +4443,318 @@
       <c r="C30" s="125" t="s">
         <v>133</v>
       </c>
-      <c r="D30" s="215"/>
-      <c r="E30" s="216"/>
-      <c r="F30" s="216"/>
-      <c r="G30" s="217"/>
+      <c r="D30" s="271"/>
+      <c r="E30" s="272"/>
+      <c r="F30" s="272"/>
+      <c r="G30" s="273"/>
       <c r="H30" s="6"/>
-      <c r="I30" s="249" t="s">
+      <c r="I30" s="194" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="173" t="s">
+      <c r="J30" s="230" t="s">
         <v>59</v>
       </c>
-      <c r="K30" s="174"/>
-      <c r="L30" s="174"/>
-      <c r="M30" s="174"/>
-      <c r="N30" s="175"/>
+      <c r="K30" s="231"/>
+      <c r="L30" s="231"/>
+      <c r="M30" s="231"/>
+      <c r="N30" s="232"/>
     </row>
     <row r="31" spans="2:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="218" t="s">
+      <c r="B31" s="274" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="183"/>
-      <c r="D31" s="183"/>
-      <c r="E31" s="183"/>
-      <c r="F31" s="183"/>
-      <c r="G31" s="168"/>
+      <c r="C31" s="242"/>
+      <c r="D31" s="242"/>
+      <c r="E31" s="242"/>
+      <c r="F31" s="242"/>
+      <c r="G31" s="192"/>
       <c r="H31" s="6"/>
-      <c r="I31" s="250"/>
-      <c r="J31" s="176"/>
-      <c r="K31" s="177"/>
-      <c r="L31" s="177"/>
-      <c r="M31" s="177"/>
-      <c r="N31" s="178"/>
+      <c r="I31" s="195"/>
+      <c r="J31" s="233"/>
+      <c r="K31" s="234"/>
+      <c r="L31" s="234"/>
+      <c r="M31" s="234"/>
+      <c r="N31" s="235"/>
     </row>
     <row r="32" spans="2:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="260" t="s">
+      <c r="B32" s="173" t="s">
         <v>134</v>
       </c>
-      <c r="C32" s="261"/>
-      <c r="D32" s="261"/>
-      <c r="E32" s="261"/>
-      <c r="F32" s="261"/>
-      <c r="G32" s="262"/>
+      <c r="C32" s="174"/>
+      <c r="D32" s="174"/>
+      <c r="E32" s="174"/>
+      <c r="F32" s="174"/>
+      <c r="G32" s="175"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="249" t="s">
+      <c r="I32" s="194" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="173" t="s">
+      <c r="J32" s="230" t="s">
         <v>142</v>
       </c>
-      <c r="K32" s="174"/>
-      <c r="L32" s="174"/>
-      <c r="M32" s="174"/>
-      <c r="N32" s="175"/>
+      <c r="K32" s="231"/>
+      <c r="L32" s="231"/>
+      <c r="M32" s="231"/>
+      <c r="N32" s="232"/>
     </row>
     <row r="33" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="218" t="s">
+      <c r="B33" s="274" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="183"/>
-      <c r="D33" s="183"/>
-      <c r="E33" s="183"/>
-      <c r="F33" s="183"/>
-      <c r="G33" s="168"/>
+      <c r="C33" s="242"/>
+      <c r="D33" s="242"/>
+      <c r="E33" s="242"/>
+      <c r="F33" s="242"/>
+      <c r="G33" s="192"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="250"/>
-      <c r="J33" s="176"/>
-      <c r="K33" s="177"/>
-      <c r="L33" s="177"/>
-      <c r="M33" s="177"/>
-      <c r="N33" s="178"/>
+      <c r="I33" s="195"/>
+      <c r="J33" s="233"/>
+      <c r="K33" s="234"/>
+      <c r="L33" s="234"/>
+      <c r="M33" s="234"/>
+      <c r="N33" s="235"/>
     </row>
     <row r="34" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="219" t="s">
+      <c r="B34" s="275" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="220"/>
-      <c r="D34" s="220"/>
-      <c r="E34" s="220"/>
-      <c r="F34" s="220"/>
-      <c r="G34" s="221"/>
+      <c r="C34" s="276"/>
+      <c r="D34" s="276"/>
+      <c r="E34" s="276"/>
+      <c r="F34" s="276"/>
+      <c r="G34" s="277"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="251" t="s">
+      <c r="I34" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="J34" s="161" t="s">
+      <c r="J34" s="253" t="s">
         <v>60</v>
       </c>
-      <c r="K34" s="162"/>
-      <c r="L34" s="162"/>
-      <c r="M34" s="162"/>
-      <c r="N34" s="194"/>
+      <c r="K34" s="254"/>
+      <c r="L34" s="254"/>
+      <c r="M34" s="254"/>
+      <c r="N34" s="255"/>
     </row>
     <row r="35" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="263" t="s">
+      <c r="B35" s="188" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="264"/>
-      <c r="D35" s="264"/>
-      <c r="E35" s="265"/>
-      <c r="F35" s="167" t="s">
+      <c r="C35" s="189"/>
+      <c r="D35" s="189"/>
+      <c r="E35" s="190"/>
+      <c r="F35" s="191" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="168"/>
+      <c r="G35" s="192"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="252"/>
-      <c r="J35" s="164"/>
-      <c r="K35" s="165"/>
-      <c r="L35" s="165"/>
-      <c r="M35" s="165"/>
-      <c r="N35" s="195"/>
+      <c r="I35" s="197"/>
+      <c r="J35" s="256"/>
+      <c r="K35" s="257"/>
+      <c r="L35" s="257"/>
+      <c r="M35" s="257"/>
+      <c r="N35" s="258"/>
       <c r="P35" s="58"/>
     </row>
     <row r="36" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="257" t="s">
+      <c r="B36" s="183" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="258"/>
-      <c r="D36" s="258"/>
-      <c r="E36" s="259"/>
-      <c r="F36" s="141" t="s">
+      <c r="C36" s="184"/>
+      <c r="D36" s="184"/>
+      <c r="E36" s="185"/>
+      <c r="F36" s="186" t="s">
         <v>137</v>
       </c>
-      <c r="G36" s="143"/>
+      <c r="G36" s="187"/>
       <c r="H36" s="6"/>
       <c r="I36" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="173" t="s">
+      <c r="J36" s="230" t="s">
         <v>61</v>
       </c>
-      <c r="K36" s="174"/>
-      <c r="L36" s="196"/>
-      <c r="M36" s="198" t="s">
+      <c r="K36" s="231"/>
+      <c r="L36" s="259"/>
+      <c r="M36" s="228" t="s">
         <v>19</v>
       </c>
-      <c r="N36" s="199"/>
+      <c r="N36" s="261"/>
     </row>
     <row r="37" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="218" t="s">
+      <c r="B37" s="274" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="183"/>
-      <c r="D37" s="183"/>
-      <c r="E37" s="222"/>
-      <c r="F37" s="167" t="s">
+      <c r="C37" s="242"/>
+      <c r="D37" s="242"/>
+      <c r="E37" s="278"/>
+      <c r="F37" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="168"/>
+      <c r="G37" s="192"/>
       <c r="H37" s="6"/>
       <c r="I37" s="126"/>
-      <c r="J37" s="176"/>
-      <c r="K37" s="177"/>
-      <c r="L37" s="197"/>
-      <c r="M37" s="200">
+      <c r="J37" s="233"/>
+      <c r="K37" s="234"/>
+      <c r="L37" s="260"/>
+      <c r="M37" s="262">
         <v>67174</v>
       </c>
-      <c r="N37" s="201"/>
+      <c r="N37" s="263"/>
     </row>
     <row r="38" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="253" t="s">
+      <c r="B38" s="224" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="142"/>
-      <c r="D38" s="142"/>
-      <c r="E38" s="254"/>
-      <c r="F38" s="141" t="s">
+      <c r="C38" s="225"/>
+      <c r="D38" s="225"/>
+      <c r="E38" s="226"/>
+      <c r="F38" s="186" t="s">
         <v>139</v>
       </c>
-      <c r="G38" s="143"/>
+      <c r="G38" s="187"/>
       <c r="H38" s="6"/>
-      <c r="I38" s="249" t="s">
+      <c r="I38" s="194" t="s">
         <v>21</v>
       </c>
-      <c r="J38" s="161" t="s">
+      <c r="J38" s="253" t="s">
         <v>62</v>
       </c>
-      <c r="K38" s="162"/>
-      <c r="L38" s="163"/>
-      <c r="M38" s="167" t="s">
+      <c r="K38" s="254"/>
+      <c r="L38" s="286"/>
+      <c r="M38" s="191" t="s">
         <v>40</v>
       </c>
-      <c r="N38" s="168"/>
+      <c r="N38" s="192"/>
     </row>
     <row r="39" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="255" t="s">
+      <c r="B39" s="227" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="198"/>
-      <c r="D39" s="256"/>
-      <c r="E39" s="167" t="s">
+      <c r="C39" s="228"/>
+      <c r="D39" s="229"/>
+      <c r="E39" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="183"/>
-      <c r="G39" s="168"/>
+      <c r="F39" s="242"/>
+      <c r="G39" s="192"/>
       <c r="H39" s="6"/>
-      <c r="I39" s="250"/>
-      <c r="J39" s="164"/>
-      <c r="K39" s="165"/>
-      <c r="L39" s="166"/>
-      <c r="M39" s="141" t="s">
+      <c r="I39" s="195"/>
+      <c r="J39" s="256"/>
+      <c r="K39" s="257"/>
+      <c r="L39" s="287"/>
+      <c r="M39" s="186" t="s">
         <v>23</v>
       </c>
-      <c r="N39" s="143"/>
+      <c r="N39" s="187"/>
     </row>
     <row r="40" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="179" t="s">
+      <c r="B40" s="236" t="s">
         <v>140</v>
       </c>
-      <c r="C40" s="180"/>
-      <c r="D40" s="181"/>
-      <c r="E40" s="184" t="s">
+      <c r="C40" s="237"/>
+      <c r="D40" s="238"/>
+      <c r="E40" s="243" t="s">
         <v>141</v>
       </c>
-      <c r="F40" s="185"/>
-      <c r="G40" s="186"/>
-      <c r="I40" s="249" t="s">
+      <c r="F40" s="244"/>
+      <c r="G40" s="245"/>
+      <c r="I40" s="194" t="s">
         <v>42</v>
       </c>
-      <c r="J40" s="202" t="s">
+      <c r="J40" s="264" t="s">
         <v>63</v>
       </c>
-      <c r="K40" s="203"/>
-      <c r="L40" s="203"/>
-      <c r="M40" s="203"/>
-      <c r="N40" s="204"/>
+      <c r="K40" s="265"/>
+      <c r="L40" s="265"/>
+      <c r="M40" s="265"/>
+      <c r="N40" s="266"/>
     </row>
     <row r="41" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="171"/>
-      <c r="C41" s="182"/>
-      <c r="D41" s="172"/>
-      <c r="E41" s="187"/>
-      <c r="F41" s="188"/>
-      <c r="G41" s="189"/>
-      <c r="I41" s="250"/>
-      <c r="J41" s="205"/>
-      <c r="K41" s="200"/>
-      <c r="L41" s="200"/>
-      <c r="M41" s="200"/>
-      <c r="N41" s="201"/>
+      <c r="B41" s="239"/>
+      <c r="C41" s="240"/>
+      <c r="D41" s="241"/>
+      <c r="E41" s="246"/>
+      <c r="F41" s="247"/>
+      <c r="G41" s="248"/>
+      <c r="I41" s="195"/>
+      <c r="J41" s="267"/>
+      <c r="K41" s="262"/>
+      <c r="L41" s="262"/>
+      <c r="M41" s="262"/>
+      <c r="N41" s="263"/>
     </row>
     <row r="42" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="229" t="s">
+      <c r="B42" s="298" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="230"/>
-      <c r="D42" s="225" t="s">
+      <c r="C42" s="299"/>
+      <c r="D42" s="220" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="226"/>
-      <c r="F42" s="223" t="s">
+      <c r="E42" s="221"/>
+      <c r="F42" s="218" t="s">
         <v>126</v>
       </c>
-      <c r="G42" s="224"/>
-      <c r="I42" s="169" t="s">
+      <c r="G42" s="219"/>
+      <c r="I42" s="288" t="s">
         <v>43</v>
       </c>
-      <c r="J42" s="170"/>
-      <c r="K42" s="206" t="s">
+      <c r="J42" s="289"/>
+      <c r="K42" s="290" t="s">
         <v>44</v>
       </c>
-      <c r="L42" s="207"/>
-      <c r="M42" s="206" t="s">
+      <c r="L42" s="291"/>
+      <c r="M42" s="290" t="s">
         <v>45</v>
       </c>
-      <c r="N42" s="208"/>
+      <c r="N42" s="292"/>
     </row>
     <row r="43" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="227" t="s">
+      <c r="B43" s="296" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="228"/>
-      <c r="D43" s="148" t="s">
+      <c r="C43" s="297"/>
+      <c r="D43" s="222" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="149"/>
-      <c r="F43" s="146" t="s">
+      <c r="E43" s="223"/>
+      <c r="F43" s="216" t="s">
         <v>130</v>
       </c>
-      <c r="G43" s="147"/>
-      <c r="I43" s="171"/>
-      <c r="J43" s="172"/>
-      <c r="K43" s="209" t="s">
+      <c r="G43" s="217"/>
+      <c r="I43" s="239"/>
+      <c r="J43" s="241"/>
+      <c r="K43" s="293" t="s">
         <v>46</v>
       </c>
-      <c r="L43" s="210"/>
-      <c r="M43" s="209" t="s">
+      <c r="L43" s="294"/>
+      <c r="M43" s="293" t="s">
         <v>27</v>
       </c>
-      <c r="N43" s="211"/>
+      <c r="N43" s="295"/>
     </row>
     <row r="44" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="160" t="s">
+      <c r="B44" s="285" t="s">
         <v>143</v>
       </c>
-      <c r="C44" s="160"/>
-      <c r="D44" s="160"/>
-      <c r="E44" s="160"/>
+      <c r="C44" s="285"/>
+      <c r="D44" s="285"/>
+      <c r="E44" s="285"/>
     </row>
     <row r="45" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="133" t="s">
         <v>151</v>
       </c>
-      <c r="C45" s="154" t="s">
+      <c r="C45" s="279" t="s">
         <v>144</v>
       </c>
-      <c r="D45" s="155"/>
-      <c r="E45" s="156"/>
-      <c r="F45" s="154" t="s">
+      <c r="D45" s="280"/>
+      <c r="E45" s="281"/>
+      <c r="F45" s="279" t="s">
         <v>148</v>
       </c>
-      <c r="G45" s="155"/>
-      <c r="H45" s="156"/>
+      <c r="G45" s="280"/>
+      <c r="H45" s="281"/>
       <c r="I45" s="131" t="s">
         <v>12</v>
       </c>
@@ -4759,11 +4764,11 @@
       <c r="K45" s="134" t="s">
         <v>146</v>
       </c>
-      <c r="L45" s="157" t="s">
+      <c r="L45" s="282" t="s">
         <v>147</v>
       </c>
-      <c r="M45" s="158"/>
-      <c r="N45" s="159"/>
+      <c r="M45" s="283"/>
+      <c r="N45" s="284"/>
     </row>
     <row r="46" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="132"/>
@@ -4857,53 +4862,33 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="M26:N27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="C27:G28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="J38:L39"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="I42:J43"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="J30:N31"/>
     <mergeCell ref="B40:D41"/>
     <mergeCell ref="E39:G39"/>
@@ -4920,36 +4905,56 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="L45:N45"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="J38:L39"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="I42:J43"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="M26:N27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="C27:G28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B14:G14"/>
   </mergeCells>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
@@ -5010,18 +5015,18 @@
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="305" t="s">
+      <c r="B2" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="306"/>
-      <c r="D2" s="306"/>
-      <c r="E2" s="306"/>
-      <c r="F2" s="306"/>
-      <c r="G2" s="306"/>
-      <c r="H2" s="306"/>
-      <c r="I2" s="306"/>
-      <c r="J2" s="306"/>
-      <c r="K2" s="307"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="146"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -5078,12 +5083,12 @@
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="403" t="s">
+      <c r="J4" s="332" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="306"/>
-      <c r="L4" s="306"/>
-      <c r="M4" s="307"/>
+      <c r="K4" s="145"/>
+      <c r="L4" s="145"/>
+      <c r="M4" s="146"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -5099,14 +5104,14 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="404" t="s">
+      <c r="A5" s="333" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="405"/>
-      <c r="C5" s="406"/>
-      <c r="D5" s="407"/>
-      <c r="E5" s="306"/>
-      <c r="F5" s="307"/>
+      <c r="B5" s="334"/>
+      <c r="C5" s="335"/>
+      <c r="D5" s="336"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="146"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -5129,23 +5134,23 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="408">
+      <c r="A6" s="337">
         <v>44008</v>
       </c>
-      <c r="B6" s="390"/>
-      <c r="C6" s="393"/>
-      <c r="D6" s="409"/>
-      <c r="E6" s="306"/>
-      <c r="F6" s="307"/>
+      <c r="B6" s="338"/>
+      <c r="C6" s="339"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="146"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="381" t="s">
+      <c r="I6" s="341" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="410"/>
-      <c r="K6" s="410"/>
-      <c r="L6" s="410"/>
-      <c r="M6" s="411"/>
+      <c r="J6" s="342"/>
+      <c r="K6" s="342"/>
+      <c r="L6" s="342"/>
+      <c r="M6" s="343"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -5162,8 +5167,8 @@
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="412"/>
-      <c r="C7" s="382"/>
+      <c r="B7" s="344"/>
+      <c r="C7" s="345"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -5189,23 +5194,23 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="319" t="s">
+      <c r="A8" s="136" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="405"/>
-      <c r="C8" s="405"/>
-      <c r="D8" s="405"/>
-      <c r="E8" s="405"/>
-      <c r="F8" s="406"/>
+      <c r="B8" s="334"/>
+      <c r="C8" s="334"/>
+      <c r="D8" s="334"/>
+      <c r="E8" s="334"/>
+      <c r="F8" s="335"/>
       <c r="G8" s="6"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="319" t="s">
+      <c r="I8" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="405"/>
-      <c r="K8" s="405"/>
-      <c r="L8" s="405"/>
-      <c r="M8" s="406"/>
+      <c r="J8" s="334"/>
+      <c r="K8" s="334"/>
+      <c r="L8" s="334"/>
+      <c r="M8" s="335"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -5221,23 +5226,23 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="396" t="s">
+      <c r="A9" s="346" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="348"/>
-      <c r="C9" s="348"/>
-      <c r="D9" s="348"/>
-      <c r="E9" s="348"/>
-      <c r="F9" s="346"/>
+      <c r="B9" s="347"/>
+      <c r="C9" s="347"/>
+      <c r="D9" s="347"/>
+      <c r="E9" s="347"/>
+      <c r="F9" s="348"/>
       <c r="G9" s="6"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="413" t="s">
+      <c r="I9" s="349" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="348"/>
-      <c r="K9" s="348"/>
-      <c r="L9" s="348"/>
-      <c r="M9" s="346"/>
+      <c r="J9" s="347"/>
+      <c r="K9" s="347"/>
+      <c r="L9" s="347"/>
+      <c r="M9" s="348"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -5253,25 +5258,25 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="302" t="s">
+      <c r="A10" s="202" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="360"/>
-      <c r="C10" s="360"/>
-      <c r="D10" s="340"/>
-      <c r="E10" s="402" t="s">
+      <c r="B10" s="328"/>
+      <c r="C10" s="328"/>
+      <c r="D10" s="329"/>
+      <c r="E10" s="330" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="341"/>
+      <c r="F10" s="331"/>
       <c r="G10" s="5"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="302" t="s">
+      <c r="I10" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="360"/>
-      <c r="K10" s="360"/>
-      <c r="L10" s="360"/>
-      <c r="M10" s="341"/>
+      <c r="J10" s="328"/>
+      <c r="K10" s="328"/>
+      <c r="L10" s="328"/>
+      <c r="M10" s="331"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -5287,25 +5292,25 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="396" t="s">
+      <c r="A11" s="346" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="348"/>
-      <c r="C11" s="348"/>
-      <c r="D11" s="349"/>
-      <c r="E11" s="398" t="s">
+      <c r="B11" s="347"/>
+      <c r="C11" s="347"/>
+      <c r="D11" s="350"/>
+      <c r="E11" s="352" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="346"/>
+      <c r="F11" s="348"/>
       <c r="G11" s="5"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="389" t="s">
+      <c r="I11" s="353" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="390"/>
-      <c r="K11" s="390"/>
-      <c r="L11" s="390"/>
-      <c r="M11" s="393"/>
+      <c r="J11" s="338"/>
+      <c r="K11" s="338"/>
+      <c r="L11" s="338"/>
+      <c r="M11" s="339"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -5321,14 +5326,14 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="302" t="s">
+      <c r="A12" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="360"/>
-      <c r="C12" s="360"/>
-      <c r="D12" s="360"/>
-      <c r="E12" s="360"/>
-      <c r="F12" s="341"/>
+      <c r="B12" s="328"/>
+      <c r="C12" s="328"/>
+      <c r="D12" s="328"/>
+      <c r="E12" s="328"/>
+      <c r="F12" s="331"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7" t="s">
         <v>12</v>
@@ -5363,14 +5368,14 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="322" t="s">
+      <c r="A13" s="139" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="348"/>
-      <c r="C13" s="348"/>
-      <c r="D13" s="348"/>
-      <c r="E13" s="348"/>
-      <c r="F13" s="346"/>
+      <c r="B13" s="347"/>
+      <c r="C13" s="347"/>
+      <c r="D13" s="347"/>
+      <c r="E13" s="347"/>
+      <c r="F13" s="348"/>
       <c r="G13" s="6"/>
       <c r="H13" s="9">
         <v>1</v>
@@ -5405,16 +5410,16 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="302" t="s">
+      <c r="A14" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="360"/>
-      <c r="C14" s="360"/>
-      <c r="D14" s="340"/>
-      <c r="E14" s="399" t="s">
+      <c r="B14" s="328"/>
+      <c r="C14" s="328"/>
+      <c r="D14" s="329"/>
+      <c r="E14" s="354" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="341"/>
+      <c r="F14" s="331"/>
       <c r="G14" s="6"/>
       <c r="H14" s="9"/>
       <c r="I14" s="13"/>
@@ -5437,16 +5442,16 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="396" t="s">
+      <c r="A15" s="346" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="348"/>
-      <c r="C15" s="348"/>
-      <c r="D15" s="349"/>
-      <c r="E15" s="400" t="s">
+      <c r="B15" s="347"/>
+      <c r="C15" s="347"/>
+      <c r="D15" s="350"/>
+      <c r="E15" s="355" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="346"/>
+      <c r="F15" s="348"/>
       <c r="G15" s="6"/>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
@@ -5469,14 +5474,14 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="401" t="s">
+      <c r="A16" s="356" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="360"/>
-      <c r="C16" s="360"/>
-      <c r="D16" s="360"/>
-      <c r="E16" s="360"/>
-      <c r="F16" s="341"/>
+      <c r="B16" s="328"/>
+      <c r="C16" s="328"/>
+      <c r="D16" s="328"/>
+      <c r="E16" s="328"/>
+      <c r="F16" s="331"/>
       <c r="G16" s="5"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -5527,16 +5532,16 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="302" t="s">
+      <c r="A18" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="360"/>
-      <c r="C18" s="360"/>
-      <c r="D18" s="340"/>
-      <c r="E18" s="399" t="s">
+      <c r="B18" s="328"/>
+      <c r="C18" s="328"/>
+      <c r="D18" s="329"/>
+      <c r="E18" s="354" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="341"/>
+      <c r="F18" s="331"/>
       <c r="G18" s="6"/>
       <c r="H18" s="25"/>
       <c r="I18" s="22"/>
@@ -5559,16 +5564,16 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="396" t="s">
+      <c r="A19" s="346" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="348"/>
-      <c r="C19" s="348"/>
-      <c r="D19" s="349"/>
-      <c r="E19" s="397" t="s">
+      <c r="B19" s="347"/>
+      <c r="C19" s="347"/>
+      <c r="D19" s="350"/>
+      <c r="E19" s="351" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="346"/>
+      <c r="F19" s="348"/>
       <c r="G19" s="6"/>
       <c r="H19" s="1"/>
       <c r="I19" s="2"/>
@@ -5591,27 +5596,27 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="380" t="s">
+      <c r="A20" s="357" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="360"/>
-      <c r="C20" s="360"/>
-      <c r="D20" s="340"/>
+      <c r="B20" s="328"/>
+      <c r="C20" s="328"/>
+      <c r="D20" s="329"/>
       <c r="E20" s="28" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="381" t="s">
+      <c r="H20" s="341" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="382"/>
-      <c r="J20" s="383" t="s">
+      <c r="I20" s="345"/>
+      <c r="J20" s="358" t="s">
         <v>27</v>
       </c>
-      <c r="K20" s="385"/>
-      <c r="L20" s="372"/>
-      <c r="M20" s="375"/>
+      <c r="K20" s="360"/>
+      <c r="L20" s="361"/>
+      <c r="M20" s="362"/>
       <c r="N20" s="1"/>
       <c r="O20" s="30"/>
       <c r="P20" s="1"/>
@@ -5627,25 +5632,25 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="389" t="s">
+      <c r="A21" s="353" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="390"/>
-      <c r="C21" s="390"/>
-      <c r="D21" s="391"/>
-      <c r="E21" s="392">
+      <c r="B21" s="338"/>
+      <c r="C21" s="338"/>
+      <c r="D21" s="366"/>
+      <c r="E21" s="367">
         <v>8115447431</v>
       </c>
-      <c r="F21" s="393"/>
+      <c r="F21" s="339"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="394" t="s">
+      <c r="H21" s="368" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="395"/>
-      <c r="J21" s="384"/>
-      <c r="K21" s="386"/>
-      <c r="L21" s="387"/>
-      <c r="M21" s="388"/>
+      <c r="I21" s="369"/>
+      <c r="J21" s="359"/>
+      <c r="K21" s="363"/>
+      <c r="L21" s="364"/>
+      <c r="M21" s="365"/>
       <c r="N21" s="1"/>
       <c r="O21" s="26"/>
       <c r="P21" s="1"/>
@@ -5668,15 +5673,15 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="369" t="s">
+      <c r="H22" s="370" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="371" t="s">
+      <c r="I22" s="372" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="372"/>
-      <c r="K22" s="372"/>
-      <c r="L22" s="372"/>
+      <c r="J22" s="361"/>
+      <c r="K22" s="361"/>
+      <c r="L22" s="361"/>
       <c r="M22" s="373"/>
       <c r="N22" s="1"/>
       <c r="O22" s="26"/>
@@ -5693,23 +5698,23 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="325" t="s">
+      <c r="A23" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="374" t="s">
+      <c r="B23" s="378" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="372"/>
-      <c r="D23" s="372"/>
-      <c r="E23" s="372"/>
-      <c r="F23" s="375"/>
+      <c r="C23" s="361"/>
+      <c r="D23" s="361"/>
+      <c r="E23" s="361"/>
+      <c r="F23" s="362"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="370"/>
-      <c r="I23" s="356"/>
-      <c r="J23" s="357"/>
-      <c r="K23" s="357"/>
-      <c r="L23" s="357"/>
-      <c r="M23" s="363"/>
+      <c r="H23" s="371"/>
+      <c r="I23" s="374"/>
+      <c r="J23" s="375"/>
+      <c r="K23" s="375"/>
+      <c r="L23" s="375"/>
+      <c r="M23" s="376"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -5725,23 +5730,23 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="352"/>
-      <c r="B24" s="356"/>
-      <c r="C24" s="357"/>
-      <c r="D24" s="357"/>
-      <c r="E24" s="357"/>
-      <c r="F24" s="358"/>
+      <c r="A24" s="377"/>
+      <c r="B24" s="374"/>
+      <c r="C24" s="375"/>
+      <c r="D24" s="375"/>
+      <c r="E24" s="375"/>
+      <c r="F24" s="379"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="351" t="s">
+      <c r="H24" s="380" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="376" t="s">
+      <c r="I24" s="381" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="354"/>
-      <c r="K24" s="354"/>
-      <c r="L24" s="354"/>
-      <c r="M24" s="355"/>
+      <c r="J24" s="382"/>
+      <c r="K24" s="382"/>
+      <c r="L24" s="382"/>
+      <c r="M24" s="383"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -5761,19 +5766,19 @@
         <v>33</v>
       </c>
       <c r="B25" s="32"/>
-      <c r="C25" s="377" t="s">
+      <c r="C25" s="384" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="378"/>
-      <c r="E25" s="378"/>
-      <c r="F25" s="379"/>
+      <c r="D25" s="385"/>
+      <c r="E25" s="385"/>
+      <c r="F25" s="386"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="352"/>
-      <c r="I25" s="356"/>
-      <c r="J25" s="357"/>
-      <c r="K25" s="357"/>
-      <c r="L25" s="357"/>
-      <c r="M25" s="358"/>
+      <c r="H25" s="377"/>
+      <c r="I25" s="374"/>
+      <c r="J25" s="375"/>
+      <c r="K25" s="375"/>
+      <c r="L25" s="375"/>
+      <c r="M25" s="379"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -5800,16 +5805,16 @@
       <c r="E26" s="35"/>
       <c r="F26" s="36"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="351" t="s">
+      <c r="H26" s="380" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="362" t="s">
+      <c r="I26" s="387" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="354"/>
-      <c r="K26" s="354"/>
-      <c r="L26" s="354"/>
-      <c r="M26" s="355"/>
+      <c r="J26" s="382"/>
+      <c r="K26" s="382"/>
+      <c r="L26" s="382"/>
+      <c r="M26" s="383"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -5825,21 +5830,21 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="367" t="s">
+      <c r="A27" s="388" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="360"/>
-      <c r="C27" s="360"/>
-      <c r="D27" s="360"/>
-      <c r="E27" s="360"/>
-      <c r="F27" s="341"/>
+      <c r="B27" s="328"/>
+      <c r="C27" s="328"/>
+      <c r="D27" s="328"/>
+      <c r="E27" s="328"/>
+      <c r="F27" s="331"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="352"/>
-      <c r="I27" s="357"/>
-      <c r="J27" s="357"/>
-      <c r="K27" s="357"/>
-      <c r="L27" s="357"/>
-      <c r="M27" s="358"/>
+      <c r="H27" s="377"/>
+      <c r="I27" s="375"/>
+      <c r="J27" s="375"/>
+      <c r="K27" s="375"/>
+      <c r="L27" s="375"/>
+      <c r="M27" s="379"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -5855,25 +5860,25 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="322" t="s">
+      <c r="A28" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="348"/>
-      <c r="C28" s="348"/>
-      <c r="D28" s="348"/>
-      <c r="E28" s="348"/>
-      <c r="F28" s="346"/>
+      <c r="B28" s="347"/>
+      <c r="C28" s="347"/>
+      <c r="D28" s="347"/>
+      <c r="E28" s="347"/>
+      <c r="F28" s="348"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="368" t="s">
+      <c r="H28" s="389" t="s">
         <v>36</v>
       </c>
-      <c r="I28" s="366" t="s">
+      <c r="I28" s="390" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="354"/>
-      <c r="K28" s="354"/>
-      <c r="L28" s="354"/>
-      <c r="M28" s="355"/>
+      <c r="J28" s="382"/>
+      <c r="K28" s="382"/>
+      <c r="L28" s="382"/>
+      <c r="M28" s="383"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -5889,21 +5894,21 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="367" t="s">
+      <c r="A29" s="388" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="360"/>
-      <c r="C29" s="360"/>
-      <c r="D29" s="360"/>
-      <c r="E29" s="360"/>
-      <c r="F29" s="341"/>
+      <c r="B29" s="328"/>
+      <c r="C29" s="328"/>
+      <c r="D29" s="328"/>
+      <c r="E29" s="328"/>
+      <c r="F29" s="331"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="352"/>
-      <c r="I29" s="357"/>
-      <c r="J29" s="357"/>
-      <c r="K29" s="357"/>
-      <c r="L29" s="357"/>
-      <c r="M29" s="358"/>
+      <c r="H29" s="377"/>
+      <c r="I29" s="375"/>
+      <c r="J29" s="375"/>
+      <c r="K29" s="375"/>
+      <c r="L29" s="375"/>
+      <c r="M29" s="379"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -5919,24 +5924,24 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="347" t="s">
+      <c r="A30" s="395" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="348"/>
-      <c r="C30" s="348"/>
-      <c r="D30" s="348"/>
-      <c r="E30" s="348"/>
-      <c r="F30" s="346"/>
+      <c r="B30" s="347"/>
+      <c r="C30" s="347"/>
+      <c r="D30" s="347"/>
+      <c r="E30" s="347"/>
+      <c r="F30" s="348"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="351" t="s">
+      <c r="H30" s="380" t="s">
         <v>18</v>
       </c>
-      <c r="I30" s="362" t="s">
+      <c r="I30" s="387" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="354"/>
-      <c r="K30" s="354"/>
-      <c r="L30" s="338"/>
+      <c r="J30" s="382"/>
+      <c r="K30" s="382"/>
+      <c r="L30" s="393"/>
       <c r="M30" s="37" t="s">
         <v>19</v>
       </c>
@@ -5955,22 +5960,22 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="364" t="s">
+      <c r="A31" s="396" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="354"/>
-      <c r="C31" s="354"/>
-      <c r="D31" s="338"/>
-      <c r="E31" s="361" t="s">
+      <c r="B31" s="382"/>
+      <c r="C31" s="382"/>
+      <c r="D31" s="393"/>
+      <c r="E31" s="394" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="341"/>
+      <c r="F31" s="331"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="352"/>
-      <c r="I31" s="357"/>
-      <c r="J31" s="357"/>
-      <c r="K31" s="357"/>
-      <c r="L31" s="363"/>
+      <c r="H31" s="377"/>
+      <c r="I31" s="375"/>
+      <c r="J31" s="375"/>
+      <c r="K31" s="375"/>
+      <c r="L31" s="376"/>
       <c r="M31" s="38">
         <v>67174</v>
       </c>
@@ -5989,25 +5994,25 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="365" t="s">
+      <c r="A32" s="391" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="357"/>
-      <c r="C32" s="357"/>
-      <c r="D32" s="363"/>
-      <c r="E32" s="350">
+      <c r="B32" s="375"/>
+      <c r="C32" s="375"/>
+      <c r="D32" s="376"/>
+      <c r="E32" s="392">
         <v>31150</v>
       </c>
-      <c r="F32" s="346"/>
+      <c r="F32" s="348"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="351" t="s">
+      <c r="H32" s="380" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="366" t="s">
+      <c r="I32" s="390" t="s">
         <v>62</v>
       </c>
-      <c r="J32" s="354"/>
-      <c r="K32" s="338"/>
+      <c r="J32" s="382"/>
+      <c r="K32" s="393"/>
       <c r="L32" s="39" t="s">
         <v>40</v>
       </c>
@@ -6027,25 +6032,25 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="367" t="s">
+      <c r="A33" s="388" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="360"/>
-      <c r="C33" s="360"/>
-      <c r="D33" s="340"/>
-      <c r="E33" s="361" t="s">
+      <c r="B33" s="328"/>
+      <c r="C33" s="328"/>
+      <c r="D33" s="329"/>
+      <c r="E33" s="394" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="341"/>
+      <c r="F33" s="331"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="352"/>
-      <c r="I33" s="357"/>
-      <c r="J33" s="357"/>
-      <c r="K33" s="363"/>
-      <c r="L33" s="345" t="s">
+      <c r="H33" s="377"/>
+      <c r="I33" s="375"/>
+      <c r="J33" s="375"/>
+      <c r="K33" s="376"/>
+      <c r="L33" s="397" t="s">
         <v>23</v>
       </c>
-      <c r="M33" s="346"/>
+      <c r="M33" s="348"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -6061,27 +6066,27 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="347" t="s">
+      <c r="A34" s="395" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="348"/>
-      <c r="C34" s="348"/>
-      <c r="D34" s="349"/>
-      <c r="E34" s="350" t="s">
+      <c r="B34" s="347"/>
+      <c r="C34" s="347"/>
+      <c r="D34" s="350"/>
+      <c r="E34" s="392" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="346"/>
+      <c r="F34" s="348"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="351" t="s">
+      <c r="H34" s="380" t="s">
         <v>42</v>
       </c>
-      <c r="I34" s="353" t="s">
+      <c r="I34" s="398" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="354"/>
-      <c r="K34" s="354"/>
-      <c r="L34" s="354"/>
-      <c r="M34" s="355"/>
+      <c r="J34" s="382"/>
+      <c r="K34" s="382"/>
+      <c r="L34" s="382"/>
+      <c r="M34" s="383"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -6097,23 +6102,23 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="359" t="s">
+      <c r="A35" s="399" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="360"/>
-      <c r="C35" s="340"/>
-      <c r="D35" s="361" t="s">
+      <c r="B35" s="328"/>
+      <c r="C35" s="329"/>
+      <c r="D35" s="394" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="360"/>
-      <c r="F35" s="341"/>
+      <c r="E35" s="328"/>
+      <c r="F35" s="331"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="352"/>
-      <c r="I35" s="356"/>
-      <c r="J35" s="357"/>
-      <c r="K35" s="357"/>
-      <c r="L35" s="357"/>
-      <c r="M35" s="358"/>
+      <c r="H35" s="377"/>
+      <c r="I35" s="374"/>
+      <c r="J35" s="375"/>
+      <c r="K35" s="375"/>
+      <c r="L35" s="375"/>
+      <c r="M35" s="379"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -6129,29 +6134,29 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="327" t="s">
+      <c r="A36" s="400" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="328"/>
-      <c r="C36" s="329"/>
-      <c r="D36" s="333">
+      <c r="B36" s="401"/>
+      <c r="C36" s="402"/>
+      <c r="D36" s="406">
         <v>6142153904</v>
       </c>
-      <c r="E36" s="328"/>
-      <c r="F36" s="334"/>
+      <c r="E36" s="401"/>
+      <c r="F36" s="407"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="337" t="s">
+      <c r="H36" s="410" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="338"/>
-      <c r="J36" s="339" t="s">
+      <c r="I36" s="393"/>
+      <c r="J36" s="411" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="340"/>
-      <c r="L36" s="339" t="s">
+      <c r="K36" s="329"/>
+      <c r="L36" s="411" t="s">
         <v>45</v>
       </c>
-      <c r="M36" s="341"/>
+      <c r="M36" s="331"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -6167,23 +6172,23 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="330"/>
-      <c r="B37" s="331"/>
-      <c r="C37" s="332"/>
-      <c r="D37" s="335"/>
-      <c r="E37" s="331"/>
-      <c r="F37" s="336"/>
+      <c r="A37" s="403"/>
+      <c r="B37" s="404"/>
+      <c r="C37" s="405"/>
+      <c r="D37" s="408"/>
+      <c r="E37" s="404"/>
+      <c r="F37" s="409"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="330"/>
-      <c r="I37" s="332"/>
-      <c r="J37" s="342" t="s">
+      <c r="H37" s="403"/>
+      <c r="I37" s="405"/>
+      <c r="J37" s="412" t="s">
         <v>27</v>
       </c>
-      <c r="K37" s="343"/>
-      <c r="L37" s="342" t="s">
+      <c r="K37" s="413"/>
+      <c r="L37" s="412" t="s">
         <v>46</v>
       </c>
-      <c r="M37" s="344"/>
+      <c r="M37" s="414"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -33166,6 +33171,66 @@
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="D36:F37"/>
+    <mergeCell ref="H36:I37"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:M35"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:L31"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:K33"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:M27"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:M29"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:M23"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:F24"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:M25"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:M21"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="I10:M10"/>
@@ -33181,66 +33246,6 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:M21"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:M23"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:F24"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:M25"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:M27"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:M29"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:K33"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:L31"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:M35"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="D36:F37"/>
-    <mergeCell ref="H36:I37"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup scale="65" orientation="landscape"/>
@@ -33374,12 +33379,12 @@
       <c r="I4" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="451" t="s">
+      <c r="J4" s="457" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="452"/>
-      <c r="L4" s="452"/>
-      <c r="M4" s="453"/>
+      <c r="K4" s="458"/>
+      <c r="L4" s="458"/>
+      <c r="M4" s="459"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -33395,14 +33400,14 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="404" t="s">
+      <c r="A5" s="333" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="405"/>
-      <c r="C5" s="406"/>
-      <c r="D5" s="407"/>
-      <c r="E5" s="306"/>
-      <c r="F5" s="307"/>
+      <c r="B5" s="334"/>
+      <c r="C5" s="335"/>
+      <c r="D5" s="336"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="146"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -33425,14 +33430,14 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="408">
+      <c r="A6" s="337">
         <v>44008</v>
       </c>
-      <c r="B6" s="390"/>
-      <c r="C6" s="393"/>
-      <c r="D6" s="409"/>
-      <c r="E6" s="306"/>
-      <c r="F6" s="307"/>
+      <c r="B6" s="338"/>
+      <c r="C6" s="339"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="146"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="J6" s="82" t="s">
@@ -33457,8 +33462,8 @@
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="412"/>
-      <c r="C7" s="382"/>
+      <c r="B7" s="344"/>
+      <c r="C7" s="345"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -33483,14 +33488,14 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="319" t="s">
+      <c r="A8" s="136" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="405"/>
-      <c r="C8" s="405"/>
-      <c r="D8" s="405"/>
-      <c r="E8" s="405"/>
-      <c r="F8" s="406"/>
+      <c r="B8" s="334"/>
+      <c r="C8" s="334"/>
+      <c r="D8" s="334"/>
+      <c r="E8" s="334"/>
+      <c r="F8" s="335"/>
       <c r="G8" s="6"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -33513,23 +33518,23 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="396" t="s">
+      <c r="A9" s="346" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="348"/>
-      <c r="C9" s="348"/>
-      <c r="D9" s="348"/>
-      <c r="E9" s="348"/>
-      <c r="F9" s="346"/>
+      <c r="B9" s="347"/>
+      <c r="C9" s="347"/>
+      <c r="D9" s="347"/>
+      <c r="E9" s="347"/>
+      <c r="F9" s="348"/>
       <c r="G9" s="6"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="454" t="s">
+      <c r="I9" s="451" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="455"/>
-      <c r="K9" s="455"/>
-      <c r="L9" s="455"/>
-      <c r="M9" s="456"/>
+      <c r="J9" s="452"/>
+      <c r="K9" s="452"/>
+      <c r="L9" s="452"/>
+      <c r="M9" s="453"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -33545,23 +33550,23 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="302" t="s">
+      <c r="A10" s="202" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="360"/>
-      <c r="C10" s="360"/>
-      <c r="D10" s="340"/>
-      <c r="E10" s="402" t="s">
+      <c r="B10" s="328"/>
+      <c r="C10" s="328"/>
+      <c r="D10" s="329"/>
+      <c r="E10" s="330" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="341"/>
+      <c r="F10" s="331"/>
       <c r="G10" s="5"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="457"/>
-      <c r="J10" s="458"/>
-      <c r="K10" s="458"/>
-      <c r="L10" s="458"/>
-      <c r="M10" s="459"/>
+      <c r="I10" s="454"/>
+      <c r="J10" s="455"/>
+      <c r="K10" s="455"/>
+      <c r="L10" s="455"/>
+      <c r="M10" s="456"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -33577,25 +33582,25 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="463" t="s">
+      <c r="A11" s="428" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="464"/>
-      <c r="C11" s="464"/>
-      <c r="D11" s="465"/>
-      <c r="E11" s="466" t="s">
+      <c r="B11" s="429"/>
+      <c r="C11" s="429"/>
+      <c r="D11" s="430"/>
+      <c r="E11" s="450" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="467"/>
+      <c r="F11" s="416"/>
       <c r="G11" s="5"/>
       <c r="H11" s="57"/>
-      <c r="I11" s="302" t="s">
+      <c r="I11" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="360"/>
-      <c r="K11" s="360"/>
-      <c r="L11" s="360"/>
-      <c r="M11" s="341"/>
+      <c r="J11" s="328"/>
+      <c r="K11" s="328"/>
+      <c r="L11" s="328"/>
+      <c r="M11" s="331"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -33611,23 +33616,23 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="302" t="s">
+      <c r="A12" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="360"/>
-      <c r="C12" s="360"/>
-      <c r="D12" s="360"/>
-      <c r="E12" s="360"/>
-      <c r="F12" s="341"/>
+      <c r="B12" s="328"/>
+      <c r="C12" s="328"/>
+      <c r="D12" s="328"/>
+      <c r="E12" s="328"/>
+      <c r="F12" s="331"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="460" t="s">
+      <c r="I12" s="423" t="s">
         <v>97</v>
       </c>
-      <c r="J12" s="461"/>
-      <c r="K12" s="461"/>
-      <c r="L12" s="461"/>
-      <c r="M12" s="462"/>
+      <c r="J12" s="424"/>
+      <c r="K12" s="424"/>
+      <c r="L12" s="424"/>
+      <c r="M12" s="427"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -33643,14 +33648,14 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="478" t="s">
+      <c r="A13" s="432" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="464"/>
-      <c r="C13" s="464"/>
-      <c r="D13" s="464"/>
-      <c r="E13" s="464"/>
-      <c r="F13" s="467"/>
+      <c r="B13" s="429"/>
+      <c r="C13" s="429"/>
+      <c r="D13" s="429"/>
+      <c r="E13" s="429"/>
+      <c r="F13" s="416"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
         <v>12</v>
@@ -33685,16 +33690,16 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="302" t="s">
+      <c r="A14" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="360"/>
-      <c r="C14" s="360"/>
-      <c r="D14" s="340"/>
-      <c r="E14" s="399" t="s">
+      <c r="B14" s="328"/>
+      <c r="C14" s="328"/>
+      <c r="D14" s="329"/>
+      <c r="E14" s="354" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="341"/>
+      <c r="F14" s="331"/>
       <c r="G14" s="6"/>
       <c r="H14" s="61">
         <v>1</v>
@@ -33729,16 +33734,16 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="463" t="s">
+      <c r="A15" s="428" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="464"/>
-      <c r="C15" s="464"/>
-      <c r="D15" s="465"/>
-      <c r="E15" s="481" t="s">
+      <c r="B15" s="429"/>
+      <c r="C15" s="429"/>
+      <c r="D15" s="430"/>
+      <c r="E15" s="431" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="467"/>
+      <c r="F15" s="416"/>
       <c r="G15" s="6"/>
       <c r="H15" s="69"/>
       <c r="I15" s="69"/>
@@ -33761,14 +33766,14 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="401" t="s">
+      <c r="A16" s="356" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="360"/>
-      <c r="C16" s="360"/>
-      <c r="D16" s="360"/>
-      <c r="E16" s="360"/>
-      <c r="F16" s="341"/>
+      <c r="B16" s="328"/>
+      <c r="C16" s="328"/>
+      <c r="D16" s="328"/>
+      <c r="E16" s="328"/>
+      <c r="F16" s="331"/>
       <c r="G16" s="5"/>
       <c r="H16" s="65"/>
       <c r="I16" s="66"/>
@@ -33819,16 +33824,16 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="302" t="s">
+      <c r="A18" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="360"/>
-      <c r="C18" s="360"/>
-      <c r="D18" s="340"/>
-      <c r="E18" s="399" t="s">
+      <c r="B18" s="328"/>
+      <c r="C18" s="328"/>
+      <c r="D18" s="329"/>
+      <c r="E18" s="354" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="341"/>
+      <c r="F18" s="331"/>
       <c r="G18" s="6"/>
       <c r="H18" s="25"/>
       <c r="I18" s="22"/>
@@ -33851,16 +33856,16 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="463" t="s">
+      <c r="A19" s="428" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="464"/>
-      <c r="C19" s="464"/>
-      <c r="D19" s="465"/>
-      <c r="E19" s="482" t="s">
+      <c r="B19" s="429"/>
+      <c r="C19" s="429"/>
+      <c r="D19" s="430"/>
+      <c r="E19" s="415" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="467"/>
+      <c r="F19" s="416"/>
       <c r="G19" s="6"/>
       <c r="H19" s="1"/>
       <c r="I19" s="2"/>
@@ -33883,12 +33888,12 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="380" t="s">
+      <c r="A20" s="357" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="360"/>
-      <c r="C20" s="360"/>
-      <c r="D20" s="340"/>
+      <c r="B20" s="328"/>
+      <c r="C20" s="328"/>
+      <c r="D20" s="329"/>
       <c r="E20" s="28" t="s">
         <v>25</v>
       </c>
@@ -33897,13 +33902,13 @@
       <c r="H20" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="471" t="s">
+      <c r="I20" s="439" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="472"/>
-      <c r="K20" s="472"/>
-      <c r="L20" s="472"/>
-      <c r="M20" s="473"/>
+      <c r="J20" s="440"/>
+      <c r="K20" s="440"/>
+      <c r="L20" s="440"/>
+      <c r="M20" s="441"/>
       <c r="N20" s="1"/>
       <c r="O20" s="30"/>
       <c r="P20" s="1"/>
@@ -33919,27 +33924,27 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="460" t="s">
+      <c r="A21" s="423" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="461"/>
-      <c r="C21" s="461"/>
-      <c r="D21" s="479"/>
-      <c r="E21" s="480" t="s">
+      <c r="B21" s="424"/>
+      <c r="C21" s="424"/>
+      <c r="D21" s="425"/>
+      <c r="E21" s="426" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="462"/>
+      <c r="F21" s="427"/>
       <c r="G21" s="6"/>
       <c r="H21" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="474" t="s">
+      <c r="I21" s="442" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="475"/>
-      <c r="K21" s="475"/>
-      <c r="L21" s="475"/>
-      <c r="M21" s="476"/>
+      <c r="J21" s="443"/>
+      <c r="K21" s="443"/>
+      <c r="L21" s="443"/>
+      <c r="M21" s="444"/>
       <c r="N21" s="1"/>
       <c r="O21" s="26"/>
       <c r="P21" s="1"/>
@@ -33962,16 +33967,16 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="369" t="s">
+      <c r="H22" s="370" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="468" t="s">
+      <c r="I22" s="433" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="469"/>
-      <c r="K22" s="469"/>
-      <c r="L22" s="469"/>
-      <c r="M22" s="470"/>
+      <c r="J22" s="434"/>
+      <c r="K22" s="434"/>
+      <c r="L22" s="434"/>
+      <c r="M22" s="435"/>
       <c r="N22" s="1"/>
       <c r="O22" s="26"/>
       <c r="P22" s="1"/>
@@ -33987,23 +33992,23 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="325" t="s">
+      <c r="A23" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="374" t="s">
+      <c r="B23" s="378" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="372"/>
-      <c r="D23" s="372"/>
-      <c r="E23" s="372"/>
-      <c r="F23" s="375"/>
+      <c r="C23" s="361"/>
+      <c r="D23" s="361"/>
+      <c r="E23" s="361"/>
+      <c r="F23" s="362"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="370"/>
-      <c r="I23" s="438"/>
-      <c r="J23" s="422"/>
-      <c r="K23" s="422"/>
-      <c r="L23" s="422"/>
-      <c r="M23" s="423"/>
+      <c r="H23" s="371"/>
+      <c r="I23" s="436"/>
+      <c r="J23" s="437"/>
+      <c r="K23" s="437"/>
+      <c r="L23" s="437"/>
+      <c r="M23" s="438"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -34019,23 +34024,23 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="352"/>
-      <c r="B24" s="356"/>
-      <c r="C24" s="357"/>
-      <c r="D24" s="357"/>
-      <c r="E24" s="357"/>
-      <c r="F24" s="358"/>
+      <c r="A24" s="377"/>
+      <c r="B24" s="374"/>
+      <c r="C24" s="375"/>
+      <c r="D24" s="375"/>
+      <c r="E24" s="375"/>
+      <c r="F24" s="379"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="351" t="s">
+      <c r="H24" s="380" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="477" t="s">
+      <c r="I24" s="445" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="420"/>
-      <c r="K24" s="420"/>
-      <c r="L24" s="420"/>
-      <c r="M24" s="437"/>
+      <c r="J24" s="446"/>
+      <c r="K24" s="446"/>
+      <c r="L24" s="446"/>
+      <c r="M24" s="447"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -34055,19 +34060,19 @@
         <v>33</v>
       </c>
       <c r="B25" s="53"/>
-      <c r="C25" s="483" t="s">
+      <c r="C25" s="417" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="484"/>
-      <c r="E25" s="484"/>
-      <c r="F25" s="485"/>
+      <c r="D25" s="418"/>
+      <c r="E25" s="418"/>
+      <c r="F25" s="419"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="352"/>
-      <c r="I25" s="438"/>
-      <c r="J25" s="422"/>
-      <c r="K25" s="422"/>
-      <c r="L25" s="422"/>
-      <c r="M25" s="439"/>
+      <c r="H25" s="377"/>
+      <c r="I25" s="436"/>
+      <c r="J25" s="437"/>
+      <c r="K25" s="437"/>
+      <c r="L25" s="437"/>
+      <c r="M25" s="448"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -34089,21 +34094,21 @@
       <c r="B26" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="486"/>
-      <c r="D26" s="487"/>
-      <c r="E26" s="487"/>
-      <c r="F26" s="488"/>
+      <c r="C26" s="420"/>
+      <c r="D26" s="421"/>
+      <c r="E26" s="421"/>
+      <c r="F26" s="422"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="351" t="s">
+      <c r="H26" s="380" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="419" t="s">
+      <c r="I26" s="449" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="420"/>
-      <c r="K26" s="420"/>
-      <c r="L26" s="420"/>
-      <c r="M26" s="437"/>
+      <c r="J26" s="446"/>
+      <c r="K26" s="446"/>
+      <c r="L26" s="446"/>
+      <c r="M26" s="447"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -34119,21 +34124,21 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="367" t="s">
+      <c r="A27" s="388" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="360"/>
-      <c r="C27" s="360"/>
-      <c r="D27" s="360"/>
-      <c r="E27" s="360"/>
-      <c r="F27" s="341"/>
+      <c r="B27" s="328"/>
+      <c r="C27" s="328"/>
+      <c r="D27" s="328"/>
+      <c r="E27" s="328"/>
+      <c r="F27" s="331"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="352"/>
-      <c r="I27" s="422"/>
-      <c r="J27" s="422"/>
-      <c r="K27" s="422"/>
-      <c r="L27" s="422"/>
-      <c r="M27" s="439"/>
+      <c r="H27" s="377"/>
+      <c r="I27" s="437"/>
+      <c r="J27" s="437"/>
+      <c r="K27" s="437"/>
+      <c r="L27" s="437"/>
+      <c r="M27" s="448"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -34149,25 +34154,25 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="450" t="s">
+      <c r="A28" s="489" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="417"/>
-      <c r="C28" s="417"/>
-      <c r="D28" s="417"/>
-      <c r="E28" s="417"/>
-      <c r="F28" s="418"/>
+      <c r="B28" s="485"/>
+      <c r="C28" s="485"/>
+      <c r="D28" s="485"/>
+      <c r="E28" s="485"/>
+      <c r="F28" s="473"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="368" t="s">
+      <c r="H28" s="389" t="s">
         <v>36</v>
       </c>
-      <c r="I28" s="434" t="s">
+      <c r="I28" s="470" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="420"/>
-      <c r="K28" s="420"/>
-      <c r="L28" s="420"/>
-      <c r="M28" s="437"/>
+      <c r="J28" s="446"/>
+      <c r="K28" s="446"/>
+      <c r="L28" s="446"/>
+      <c r="M28" s="447"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -34183,21 +34188,21 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="367" t="s">
+      <c r="A29" s="388" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="360"/>
-      <c r="C29" s="360"/>
-      <c r="D29" s="360"/>
-      <c r="E29" s="360"/>
-      <c r="F29" s="341"/>
+      <c r="B29" s="328"/>
+      <c r="C29" s="328"/>
+      <c r="D29" s="328"/>
+      <c r="E29" s="328"/>
+      <c r="F29" s="331"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="352"/>
-      <c r="I29" s="422"/>
-      <c r="J29" s="422"/>
-      <c r="K29" s="422"/>
-      <c r="L29" s="422"/>
-      <c r="M29" s="439"/>
+      <c r="H29" s="377"/>
+      <c r="I29" s="437"/>
+      <c r="J29" s="437"/>
+      <c r="K29" s="437"/>
+      <c r="L29" s="437"/>
+      <c r="M29" s="448"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -34213,24 +34218,24 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="416" t="s">
+      <c r="A30" s="484" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="417"/>
-      <c r="C30" s="417"/>
-      <c r="D30" s="417"/>
-      <c r="E30" s="417"/>
-      <c r="F30" s="418"/>
+      <c r="B30" s="485"/>
+      <c r="C30" s="485"/>
+      <c r="D30" s="485"/>
+      <c r="E30" s="485"/>
+      <c r="F30" s="473"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="351" t="s">
+      <c r="H30" s="380" t="s">
         <v>18</v>
       </c>
-      <c r="I30" s="419" t="s">
+      <c r="I30" s="449" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="420"/>
-      <c r="K30" s="420"/>
-      <c r="L30" s="421"/>
+      <c r="J30" s="446"/>
+      <c r="K30" s="446"/>
+      <c r="L30" s="471"/>
       <c r="M30" s="71" t="s">
         <v>19</v>
       </c>
@@ -34249,22 +34254,22 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="364" t="s">
+      <c r="A31" s="396" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="354"/>
-      <c r="C31" s="354"/>
-      <c r="D31" s="338"/>
-      <c r="E31" s="361" t="s">
+      <c r="B31" s="382"/>
+      <c r="C31" s="382"/>
+      <c r="D31" s="393"/>
+      <c r="E31" s="394" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="341"/>
+      <c r="F31" s="331"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="352"/>
-      <c r="I31" s="422"/>
-      <c r="J31" s="422"/>
-      <c r="K31" s="422"/>
-      <c r="L31" s="423"/>
+      <c r="H31" s="377"/>
+      <c r="I31" s="437"/>
+      <c r="J31" s="437"/>
+      <c r="K31" s="437"/>
+      <c r="L31" s="438"/>
       <c r="M31" s="72">
         <v>67174</v>
       </c>
@@ -34283,25 +34288,25 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="446" t="s">
+      <c r="A32" s="481" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="447"/>
-      <c r="C32" s="447"/>
-      <c r="D32" s="448"/>
-      <c r="E32" s="435" t="s">
+      <c r="B32" s="482"/>
+      <c r="C32" s="482"/>
+      <c r="D32" s="483"/>
+      <c r="E32" s="472" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="418"/>
+      <c r="F32" s="473"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="351" t="s">
+      <c r="H32" s="380" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="434" t="s">
+      <c r="I32" s="470" t="s">
         <v>62</v>
       </c>
-      <c r="J32" s="420"/>
-      <c r="K32" s="421"/>
+      <c r="J32" s="446"/>
+      <c r="K32" s="471"/>
       <c r="L32" s="73" t="s">
         <v>40</v>
       </c>
@@ -34321,25 +34326,25 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="367" t="s">
+      <c r="A33" s="388" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="360"/>
-      <c r="C33" s="360"/>
-      <c r="D33" s="340"/>
-      <c r="E33" s="361" t="s">
+      <c r="B33" s="328"/>
+      <c r="C33" s="328"/>
+      <c r="D33" s="329"/>
+      <c r="E33" s="394" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="341"/>
+      <c r="F33" s="331"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="352"/>
-      <c r="I33" s="422"/>
-      <c r="J33" s="422"/>
-      <c r="K33" s="423"/>
-      <c r="L33" s="414" t="s">
+      <c r="H33" s="377"/>
+      <c r="I33" s="437"/>
+      <c r="J33" s="437"/>
+      <c r="K33" s="438"/>
+      <c r="L33" s="487" t="s">
         <v>23</v>
       </c>
-      <c r="M33" s="415"/>
+      <c r="M33" s="488"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -34355,27 +34360,27 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="416" t="s">
+      <c r="A34" s="484" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="417"/>
-      <c r="C34" s="417"/>
-      <c r="D34" s="449"/>
-      <c r="E34" s="435" t="s">
+      <c r="B34" s="485"/>
+      <c r="C34" s="485"/>
+      <c r="D34" s="486"/>
+      <c r="E34" s="472" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="418"/>
+      <c r="F34" s="473"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="351" t="s">
+      <c r="H34" s="380" t="s">
         <v>42</v>
       </c>
-      <c r="I34" s="436" t="s">
+      <c r="I34" s="474" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="420"/>
-      <c r="K34" s="420"/>
-      <c r="L34" s="420"/>
-      <c r="M34" s="437"/>
+      <c r="J34" s="446"/>
+      <c r="K34" s="446"/>
+      <c r="L34" s="446"/>
+      <c r="M34" s="447"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -34391,23 +34396,23 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="359" t="s">
+      <c r="A35" s="399" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="360"/>
-      <c r="C35" s="340"/>
-      <c r="D35" s="361" t="s">
+      <c r="B35" s="328"/>
+      <c r="C35" s="329"/>
+      <c r="D35" s="394" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="360"/>
-      <c r="F35" s="341"/>
+      <c r="E35" s="328"/>
+      <c r="F35" s="331"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="352"/>
-      <c r="I35" s="438"/>
-      <c r="J35" s="422"/>
-      <c r="K35" s="422"/>
-      <c r="L35" s="422"/>
-      <c r="M35" s="439"/>
+      <c r="H35" s="377"/>
+      <c r="I35" s="436"/>
+      <c r="J35" s="437"/>
+      <c r="K35" s="437"/>
+      <c r="L35" s="437"/>
+      <c r="M35" s="448"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -34423,29 +34428,29 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="424" t="s">
+      <c r="A36" s="460" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="425"/>
-      <c r="C36" s="426"/>
-      <c r="D36" s="430" t="s">
+      <c r="B36" s="461"/>
+      <c r="C36" s="462"/>
+      <c r="D36" s="466" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="425"/>
-      <c r="F36" s="431"/>
+      <c r="E36" s="461"/>
+      <c r="F36" s="467"/>
       <c r="G36" s="6"/>
       <c r="H36" s="48" t="s">
         <v>43</v>
       </c>
       <c r="I36" s="75"/>
-      <c r="J36" s="440" t="s">
+      <c r="J36" s="475" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="441"/>
-      <c r="L36" s="440" t="s">
+      <c r="K36" s="476"/>
+      <c r="L36" s="475" t="s">
         <v>45</v>
       </c>
-      <c r="M36" s="442"/>
+      <c r="M36" s="477"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -34461,23 +34466,23 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="427"/>
-      <c r="B37" s="428"/>
-      <c r="C37" s="429"/>
-      <c r="D37" s="432"/>
-      <c r="E37" s="428"/>
-      <c r="F37" s="433"/>
+      <c r="A37" s="463"/>
+      <c r="B37" s="464"/>
+      <c r="C37" s="465"/>
+      <c r="D37" s="468"/>
+      <c r="E37" s="464"/>
+      <c r="F37" s="469"/>
       <c r="G37" s="6"/>
       <c r="H37" s="47"/>
       <c r="I37" s="76"/>
-      <c r="J37" s="443" t="s">
+      <c r="J37" s="478" t="s">
         <v>69</v>
       </c>
-      <c r="K37" s="444"/>
-      <c r="L37" s="443" t="s">
+      <c r="K37" s="479"/>
+      <c r="L37" s="478" t="s">
         <v>27</v>
       </c>
-      <c r="M37" s="445"/>
+      <c r="M37" s="480"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -61458,48 +61463,18 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:F24"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="C25:F26"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="I22:M23"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="I21:M21"/>
-    <mergeCell ref="I24:M25"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:M27"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="I30:L31"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="I28:M29"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="H30:H31"/>
     <mergeCell ref="A36:C37"/>
     <mergeCell ref="D36:F37"/>
     <mergeCell ref="I32:K33"/>
@@ -61516,18 +61491,48 @@
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="I30:L31"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="I28:M29"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="I22:M23"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="I24:M25"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:M27"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:F24"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="C25:F26"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup scale="70" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>